<commit_message>
Add Exceptions and code cleaning
</commit_message>
<xml_diff>
--- a/src/test/java/Subscriptions/Data/Option_Positions_Subscription.xlsx
+++ b/src/test/java/Subscriptions/Data/Option_Positions_Subscription.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajmal.syed.LOGICIELSERVICE\eclipse-workspace\OMS_API\src\test\java\Subscriptions\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation_OMSAPI\src\test\java\Subscriptions\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D858C6-2A47-49F3-92E7-B58E490560B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D38162-BF3C-4F05-86B8-A6C980DA5DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="363" firstSheet="3" activeTab="3" xr2:uid="{A77A0332-03F7-4C79-B0EA-4DB171BB1F0C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="363" firstSheet="1" activeTab="2" xr2:uid="{A77A0332-03F7-4C79-B0EA-4DB171BB1F0C}"/>
   </bookViews>
   <sheets>
     <sheet name="SubscribeBUYOption_Positions" sheetId="10" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="265">
   <si>
     <t>Content_Type</t>
   </si>
@@ -1014,7 +1014,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1057,6 +1057,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1371,10 +1372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41536820-D56A-41BA-A388-6D13CFA1508B}">
-  <dimension ref="A1:CU2"/>
+  <dimension ref="A1:CD2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,96 +1389,82 @@
     <col min="7" max="7" width="27" style="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="30.42578125" style="14" customWidth="1"/>
-    <col min="13" max="13" width="22.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.28515625" style="14" customWidth="1"/>
-    <col min="16" max="16" width="14.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16" style="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="17.85546875" style="14" customWidth="1"/>
-    <col min="23" max="23" width="27" style="14" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="17.85546875" style="14" customWidth="1"/>
-    <col min="27" max="27" width="23.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="30.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="155.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="32" style="14" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="30.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="49.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11" style="14" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="28.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="32.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="26.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="33.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="30.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="33.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="23.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="30.42578125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="30.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="155.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="49.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="32.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="33.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="33.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="31.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="36.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="47.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="31.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="24.5703125" style="14" customWidth="1"/>
+    <col min="30" max="30" width="26" style="14" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="25" style="14" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="26.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="22.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="27.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="28.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="27.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="23.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="21.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="26.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="31.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="36.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="47.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="31.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="24.5703125" style="14" customWidth="1"/>
-    <col min="47" max="47" width="26" style="14" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="21.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="24.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="25" style="14" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="26.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="22.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="27.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="28.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="27.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="23.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="21.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="26.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="31.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="36.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="27.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="29" style="14" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="26.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="31.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="35.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="33" style="14" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="32.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="38.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="35" style="14" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="31.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="41.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="35.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="38.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="37" style="14" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="31.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="31.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="41.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="37.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="36.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="35.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="42.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="46.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="36.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="34.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="35.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="33" style="14" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="46.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="44" style="14" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="41.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="39.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="39.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="34.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="28.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="34.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="31" style="14" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="37.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="33.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="42.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="31.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="100" max="16384" width="9.140625" style="14"/>
+    <col min="43" max="43" width="36.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="27.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="29" style="14" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="26.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="31.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="35.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="33" style="14" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="32.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="38.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="35" style="14" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="31.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="41.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="35.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="38.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="37" style="14" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="31.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="31.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="41.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="37.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="36.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="35.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="42.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="46.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="36.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="34.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="35.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="33" style="14" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="46.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="44" style="14" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="41.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="39.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="39.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="34.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="28.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="34.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="31" style="14" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="37.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="33.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="42.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="31.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="83" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>153</v>
       </c>
@@ -1512,271 +1499,220 @@
         <v>159</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>152</v>
+        <v>187</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>14</v>
+        <v>168</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>227</v>
+        <v>170</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>68</v>
+        <v>171</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>70</v>
+        <v>178</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>71</v>
+        <v>179</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>72</v>
+        <v>180</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>228</v>
+        <v>181</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>229</v>
+        <v>182</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>230</v>
+        <v>183</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>232</v>
+        <v>185</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>233</v>
+        <v>186</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>234</v>
+        <v>29</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>187</v>
+        <v>31</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>169</v>
+        <v>32</v>
+      </c>
+      <c r="AE1" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>170</v>
+        <v>34</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>179</v>
+        <v>35</v>
+      </c>
+      <c r="AH1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ1" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="AK1" s="2" t="s">
-        <v>180</v>
+        <v>39</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>181</v>
+        <v>40</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>182</v>
+        <v>41</v>
       </c>
       <c r="AN1" s="2" t="s">
-        <v>183</v>
+        <v>42</v>
       </c>
       <c r="AO1" s="2" t="s">
-        <v>184</v>
+        <v>43</v>
       </c>
       <c r="AP1" s="2" t="s">
-        <v>185</v>
+        <v>146</v>
       </c>
       <c r="AQ1" s="2" t="s">
-        <v>186</v>
+        <v>44</v>
       </c>
       <c r="AR1" s="2" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="AS1" s="2" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="AT1" s="2" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="AU1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AV1" s="6" t="s">
-        <v>33</v>
+        <v>48</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="AW1" s="2" t="s">
-        <v>34</v>
+        <v>188</v>
       </c>
       <c r="AX1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AY1" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="AZ1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="BA1" s="6" t="s">
-        <v>38</v>
+        <v>189</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="BA1" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="BB1" s="2" t="s">
-        <v>39</v>
+        <v>193</v>
       </c>
       <c r="BC1" s="2" t="s">
-        <v>40</v>
+        <v>194</v>
       </c>
       <c r="BD1" s="2" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="BE1" s="2" t="s">
-        <v>42</v>
+        <v>196</v>
       </c>
       <c r="BF1" s="2" t="s">
-        <v>43</v>
+        <v>197</v>
       </c>
       <c r="BG1" s="2" t="s">
-        <v>146</v>
+        <v>198</v>
       </c>
       <c r="BH1" s="2" t="s">
-        <v>44</v>
+        <v>199</v>
       </c>
       <c r="BI1" s="2" t="s">
-        <v>45</v>
+        <v>200</v>
       </c>
       <c r="BJ1" s="2" t="s">
-        <v>46</v>
+        <v>201</v>
       </c>
       <c r="BK1" s="2" t="s">
-        <v>47</v>
+        <v>202</v>
       </c>
       <c r="BL1" s="2" t="s">
-        <v>48</v>
+        <v>203</v>
       </c>
       <c r="BM1" s="2" t="s">
-        <v>49</v>
+        <v>204</v>
       </c>
       <c r="BN1" s="2" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="BO1" s="2" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
       <c r="BP1" s="2" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c r="BQ1" s="2" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="BR1" s="2" t="s">
-        <v>192</v>
+        <v>209</v>
       </c>
       <c r="BS1" s="2" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
       <c r="BT1" s="2" t="s">
-        <v>194</v>
+        <v>211</v>
       </c>
       <c r="BU1" s="2" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
       <c r="BV1" s="2" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
       <c r="BW1" s="2" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="BX1" s="2" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="BY1" s="2" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
       <c r="BZ1" s="2" t="s">
-        <v>200</v>
+        <v>217</v>
       </c>
       <c r="CA1" s="2" t="s">
-        <v>201</v>
+        <v>75</v>
       </c>
       <c r="CB1" s="2" t="s">
-        <v>202</v>
+        <v>144</v>
       </c>
       <c r="CC1" s="2" t="s">
-        <v>203</v>
+        <v>145</v>
       </c>
       <c r="CD1" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="CE1" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="CF1" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="CG1" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="CH1" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="CI1" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="CJ1" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="CK1" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="CL1" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="CM1" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CN1" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="CO1" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="CP1" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="CQ1" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="CR1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="CS1" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="CT1" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="CU1" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>259</v>
       </c>
@@ -1810,268 +1746,217 @@
       <c r="K2" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="L2" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>162</v>
       </c>
+      <c r="M2" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="N2" s="3">
+        <v>200</v>
+      </c>
       <c r="O2" s="3" t="s">
-        <v>147</v>
+        <v>25</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>15</v>
+        <v>172</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>200</v>
       </c>
       <c r="R2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S2" s="3">
+        <v>2</v>
+      </c>
+      <c r="T2" s="3">
+        <v>1</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="W2" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="S2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="U2" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="V2" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="X2" s="3" t="s">
-        <v>15</v>
+        <v>175</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>164</v>
+        <v>93</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>165</v>
+        <v>54</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>166</v>
+        <v>55</v>
       </c>
       <c r="AB2" s="3">
         <v>200</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>162</v>
+        <v>56</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>167</v>
+        <v>57</v>
       </c>
       <c r="AE2" s="3">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>25</v>
+        <v>173</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="AH2" s="3">
-        <v>200</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>52</v>
+        <v>10</v>
+      </c>
+      <c r="AI2" s="3">
+        <v>40</v>
       </c>
       <c r="AJ2" s="3">
         <v>2</v>
       </c>
-      <c r="AK2" s="3">
+      <c r="AK2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AZ2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="BA2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="BB2" s="14">
+        <v>2</v>
+      </c>
+      <c r="BC2" s="14">
         <v>1</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="BD2" s="14">
+        <v>0</v>
+      </c>
+      <c r="BE2" s="14">
+        <v>0</v>
+      </c>
+      <c r="BF2" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="BG2" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="BH2" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="BI2" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="AM2" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS2" s="3">
-        <v>200</v>
-      </c>
-      <c r="AT2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AU2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AV2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AW2" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="AX2" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="AY2" s="3">
-        <v>10</v>
-      </c>
-      <c r="AZ2" s="3">
-        <v>40</v>
-      </c>
-      <c r="BA2" s="3">
-        <v>2</v>
-      </c>
-      <c r="BB2" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="BC2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="BD2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BE2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BF2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="BG2" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="BH2" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="BI2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BJ2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="BK2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="BL2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="BM2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="BN2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BO2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BP2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BQ2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BR2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BS2" s="14">
-        <v>2</v>
-      </c>
-      <c r="BT2" s="14">
-        <v>1</v>
-      </c>
-      <c r="BU2" s="14">
-        <v>0</v>
-      </c>
-      <c r="BV2" s="14">
-        <v>0</v>
+      <c r="BJ2" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="BK2" s="14">
+        <v>30</v>
+      </c>
+      <c r="BL2" s="14">
+        <v>209908</v>
+      </c>
+      <c r="BM2" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="BN2" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="BO2" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="BP2" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="BQ2" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="BR2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="BS2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="BT2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="BU2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="BV2" s="14" t="s">
+        <v>59</v>
       </c>
       <c r="BW2" s="14" t="s">
-        <v>174</v>
+        <v>15</v>
       </c>
       <c r="BX2" s="14" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="BY2" s="14" t="s">
-        <v>219</v>
+        <v>59</v>
       </c>
       <c r="BZ2" s="14" t="s">
         <v>173</v>
       </c>
       <c r="CA2" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="CB2" s="14">
-        <v>30</v>
-      </c>
-      <c r="CC2" s="14">
-        <v>209908</v>
+        <v>11</v>
+      </c>
+      <c r="CB2" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="CC2" s="14" t="s">
+        <v>59</v>
       </c>
       <c r="CD2" s="14" t="s">
-        <v>220</v>
-      </c>
-      <c r="CE2" s="14" t="s">
-        <v>221</v>
-      </c>
-      <c r="CF2" s="14" t="s">
-        <v>222</v>
-      </c>
-      <c r="CG2" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="CH2" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="CI2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="CJ2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="CK2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="CL2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="CM2" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="CN2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="CO2" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="CP2" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="CQ2" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="CR2" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="CS2" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="CT2" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="CU2" s="14" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2083,10 +1968,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30BCD8FC-EB92-4047-A4A0-66F914093932}">
-  <dimension ref="A1:DZ2"/>
+  <dimension ref="A1:DI2"/>
   <sheetViews>
-    <sheetView topLeftCell="BV1" workbookViewId="0">
-      <selection activeCell="BZ1" sqref="BZ1:CR2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2100,101 +1985,87 @@
     <col min="7" max="7" width="27" style="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="30.42578125" style="14" customWidth="1"/>
-    <col min="13" max="13" width="22.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.28515625" style="14" customWidth="1"/>
-    <col min="16" max="16" width="24.140625" style="14" customWidth="1"/>
-    <col min="17" max="17" width="22.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16" style="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="17.85546875" style="14" customWidth="1"/>
-    <col min="23" max="23" width="27" style="14" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="17.85546875" style="14" customWidth="1"/>
-    <col min="27" max="27" width="23.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="30.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="73.7109375" style="14" customWidth="1"/>
-    <col min="32" max="32" width="32" style="14" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="30.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="49.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11" style="14" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="28.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="32.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="26.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="33.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="30.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="33.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="23.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="31.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="31.28515625" style="14" customWidth="1"/>
-    <col min="45" max="45" width="36.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="46" max="54" width="36.7109375" style="14" customWidth="1"/>
-    <col min="55" max="55" width="42.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="47.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="31.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="24.5703125" style="14" customWidth="1"/>
-    <col min="59" max="59" width="26" style="14" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="26.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="24.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="25" style="14" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="30.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="26.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="31.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="28.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="27.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="23.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="21.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="31.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="35.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="36.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="27.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="29" style="14" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="26.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="31.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="39.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="78" max="95" width="35.42578125" style="14" customWidth="1"/>
-    <col min="96" max="96" width="39.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="33" style="14" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="32.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="38.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="35" style="14" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="31.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="41.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="35.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="38.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="37" style="14" bestFit="1" customWidth="1"/>
-    <col min="106" max="106" width="31.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="31.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="41.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="37.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="36.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="35.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="42.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="46.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="36.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="34.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="35.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="33" style="14" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="46.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="44" style="14" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="41.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="39.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="39.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="34.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="28.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="34.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="31" style="14" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="37.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="128" max="128" width="33.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="42.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="31.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="131" max="16384" width="9.140625" style="14"/>
+    <col min="10" max="11" width="30.42578125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="30.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="73.7109375" style="14" customWidth="1"/>
+    <col min="15" max="15" width="32" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="49.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="32.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="33.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="30.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="33.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="23.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="31.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="31.28515625" style="14" customWidth="1"/>
+    <col min="28" max="28" width="36.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="29" max="37" width="36.7109375" style="14" customWidth="1"/>
+    <col min="38" max="38" width="42.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="47.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="31.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="24.5703125" style="14" customWidth="1"/>
+    <col min="42" max="42" width="26" style="14" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="26.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="24.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="25" style="14" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="30.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="26.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="31.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="28.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="27.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="23.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="21.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="31.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="35.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="36.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="27.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="29" style="14" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="26.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="31.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="39.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="61" max="78" width="35.42578125" style="14" customWidth="1"/>
+    <col min="79" max="79" width="39.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="33" style="14" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="32.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="38.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="35" style="14" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="31.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="41.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="35.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="38.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="37" style="14" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="31.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="31.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="41.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="37.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="36.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="35.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="42.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="46.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="36.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="34.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="35.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="33" style="14" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="46.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="44" style="14" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="41.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="39.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="39.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="106" max="106" width="34.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="28.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="34.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="31" style="14" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="37.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="33.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="42.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="31.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="114" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:130" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:113" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>153</v>
       </c>
@@ -2229,364 +2100,313 @@
         <v>159</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>152</v>
+        <v>187</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>14</v>
+        <v>252</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>67</v>
+        <v>237</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>227</v>
+        <v>169</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>68</v>
+        <v>170</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>69</v>
+        <v>171</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>71</v>
+        <v>178</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>72</v>
+        <v>179</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>228</v>
+        <v>180</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>229</v>
+        <v>181</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>230</v>
+        <v>182</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>231</v>
+        <v>183</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>232</v>
+        <v>184</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>233</v>
+        <v>185</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>234</v>
+        <v>254</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>73</v>
+        <v>186</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>187</v>
+        <v>239</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="AE1" s="2" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>169</v>
+        <v>242</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>170</v>
+        <v>243</v>
       </c>
       <c r="AH1" s="2" t="s">
-        <v>171</v>
+        <v>244</v>
       </c>
       <c r="AI1" s="2" t="s">
-        <v>27</v>
+        <v>245</v>
       </c>
       <c r="AJ1" s="2" t="s">
-        <v>178</v>
+        <v>246</v>
       </c>
       <c r="AK1" s="2" t="s">
-        <v>179</v>
+        <v>253</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>180</v>
+        <v>247</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>181</v>
+        <v>29</v>
       </c>
       <c r="AN1" s="2" t="s">
-        <v>182</v>
+        <v>30</v>
       </c>
       <c r="AO1" s="2" t="s">
-        <v>183</v>
+        <v>31</v>
       </c>
       <c r="AP1" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>185</v>
+        <v>248</v>
+      </c>
+      <c r="AQ1" s="6" t="s">
+        <v>249</v>
       </c>
       <c r="AR1" s="2" t="s">
-        <v>254</v>
+        <v>107</v>
       </c>
       <c r="AS1" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="AU1" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>241</v>
+        <v>108</v>
+      </c>
+      <c r="AT1" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="AU1" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="AV1" s="6" t="s">
+        <v>111</v>
       </c>
       <c r="AW1" s="2" t="s">
-        <v>242</v>
+        <v>112</v>
       </c>
       <c r="AX1" s="2" t="s">
-        <v>243</v>
+        <v>113</v>
       </c>
       <c r="AY1" s="2" t="s">
-        <v>244</v>
+        <v>114</v>
       </c>
       <c r="AZ1" s="2" t="s">
-        <v>245</v>
+        <v>115</v>
       </c>
       <c r="BA1" s="2" t="s">
-        <v>246</v>
+        <v>116</v>
       </c>
       <c r="BB1" s="2" t="s">
-        <v>253</v>
+        <v>148</v>
       </c>
       <c r="BC1" s="2" t="s">
-        <v>247</v>
+        <v>117</v>
       </c>
       <c r="BD1" s="2" t="s">
-        <v>29</v>
+        <v>118</v>
       </c>
       <c r="BE1" s="2" t="s">
-        <v>30</v>
+        <v>119</v>
       </c>
       <c r="BF1" s="2" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="BG1" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="BH1" s="6" t="s">
-        <v>249</v>
+        <v>121</v>
+      </c>
+      <c r="BH1" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="BI1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="BJ1" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="BK1" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="BL1" s="6" t="s">
-        <v>110</v>
+        <v>250</v>
+      </c>
+      <c r="BJ1" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="BK1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="BL1" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="BM1" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="BN1" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="BO1" s="2" t="s">
-        <v>113</v>
+        <v>127</v>
+      </c>
+      <c r="BN1" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="BO1" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="BP1" s="2" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="BQ1" s="2" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="BR1" s="2" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="BS1" s="2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="BT1" s="2" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="BU1" s="2" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="BV1" s="2" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="BW1" s="2" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="BX1" s="2" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="BY1" s="2" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="BZ1" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="CA1" s="6" t="s">
-        <v>251</v>
+        <v>139</v>
+      </c>
+      <c r="CA1" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="CB1" s="2" t="s">
-        <v>125</v>
+        <v>188</v>
       </c>
       <c r="CC1" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="CD1" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="CE1" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="CF1" s="6" t="s">
-        <v>129</v>
+        <v>189</v>
+      </c>
+      <c r="CD1" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="CE1" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="CF1" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="CG1" s="2" t="s">
-        <v>130</v>
+        <v>193</v>
       </c>
       <c r="CH1" s="2" t="s">
-        <v>131</v>
+        <v>194</v>
       </c>
       <c r="CI1" s="2" t="s">
-        <v>132</v>
+        <v>195</v>
       </c>
       <c r="CJ1" s="2" t="s">
-        <v>133</v>
+        <v>196</v>
       </c>
       <c r="CK1" s="2" t="s">
-        <v>134</v>
+        <v>197</v>
       </c>
       <c r="CL1" s="2" t="s">
-        <v>149</v>
+        <v>198</v>
       </c>
       <c r="CM1" s="2" t="s">
-        <v>135</v>
+        <v>199</v>
       </c>
       <c r="CN1" s="2" t="s">
-        <v>136</v>
+        <v>200</v>
       </c>
       <c r="CO1" s="2" t="s">
-        <v>137</v>
+        <v>201</v>
       </c>
       <c r="CP1" s="2" t="s">
-        <v>138</v>
+        <v>202</v>
       </c>
       <c r="CQ1" s="2" t="s">
-        <v>139</v>
+        <v>203</v>
       </c>
       <c r="CR1" s="2" t="s">
-        <v>140</v>
+        <v>204</v>
       </c>
       <c r="CS1" s="2" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="CT1" s="2" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
       <c r="CU1" s="2" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c r="CV1" s="2" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="CW1" s="2" t="s">
-        <v>192</v>
+        <v>209</v>
       </c>
       <c r="CX1" s="2" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
       <c r="CY1" s="2" t="s">
-        <v>194</v>
+        <v>211</v>
       </c>
       <c r="CZ1" s="2" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
       <c r="DA1" s="2" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
       <c r="DB1" s="2" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="DC1" s="2" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="DD1" s="2" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
       <c r="DE1" s="2" t="s">
-        <v>200</v>
+        <v>217</v>
       </c>
       <c r="DF1" s="2" t="s">
-        <v>201</v>
+        <v>75</v>
       </c>
       <c r="DG1" s="2" t="s">
-        <v>202</v>
+        <v>144</v>
       </c>
       <c r="DH1" s="2" t="s">
-        <v>203</v>
+        <v>145</v>
       </c>
       <c r="DI1" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="DJ1" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="DK1" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="DL1" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="DM1" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="DN1" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="DO1" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="DP1" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="DQ1" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="DR1" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="DS1" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="DT1" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="DU1" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="DV1" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="DW1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="DX1" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="DY1" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="DZ1" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:130" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:113" s="3" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>258</v>
       </c>
@@ -2621,360 +2441,309 @@
         <v>161</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>11</v>
+        <v>162</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>17</v>
+        <v>235</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="O2" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="O2" s="3">
+        <v>200</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="R2" s="3">
+        <v>200</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T2" s="3">
+        <v>2</v>
+      </c>
+      <c r="U2" s="3">
+        <v>1</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD2" s="3">
+        <v>2</v>
+      </c>
+      <c r="AE2" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="AF2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN2" s="3">
+        <v>200</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AQ2" s="3">
+        <v>1</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="AV2" s="3">
+        <v>2</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AY2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AZ2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="BA2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="3" t="s">
+      <c r="BB2" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="BC2" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="BD2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="BE2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="BF2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="BG2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="BH2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="BI2" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="BJ2" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="BK2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="BL2" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="BM2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="BN2" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="BO2" s="3">
+        <v>2</v>
+      </c>
+      <c r="BP2" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="S2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="U2" s="16" t="s">
+      <c r="BQ2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="BR2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="BS2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="BT2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="BU2" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="BV2" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="BW2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="BX2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="BY2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="BZ2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="CA2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="CB2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CC2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CD2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CE2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CF2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CG2" s="3">
+        <v>2</v>
+      </c>
+      <c r="CH2" s="3">
+        <v>1</v>
+      </c>
+      <c r="CI2" s="3">
+        <v>0</v>
+      </c>
+      <c r="CJ2" s="3">
+        <v>0</v>
+      </c>
+      <c r="CK2" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="CL2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="CM2" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="CN2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="CO2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="CP2" s="3">
+        <v>30</v>
+      </c>
+      <c r="CQ2" s="3">
+        <v>209908</v>
+      </c>
+      <c r="CR2" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="CS2" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="CT2" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="CU2" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="CV2" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="V2" s="16" t="s">
-        <v>225</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="AB2" s="3">
-        <v>200</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="AF2" s="3">
-        <v>200</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="AI2" s="3">
-        <v>200</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK2" s="3">
-        <v>2</v>
-      </c>
-      <c r="AL2" s="3">
-        <v>1</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="AR2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="AS2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AT2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU2" s="3">
-        <v>2</v>
-      </c>
-      <c r="AV2" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="AW2" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="AX2" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="AY2" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="AZ2" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="BA2" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="BB2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="BC2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="BD2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="BE2" s="3">
-        <v>200</v>
-      </c>
-      <c r="BF2" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="BG2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="BH2" s="3">
-        <v>1</v>
-      </c>
-      <c r="BI2" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="BJ2" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="BK2" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="BL2" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="BM2" s="3">
-        <v>2</v>
-      </c>
-      <c r="BN2" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="BO2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="BP2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BQ2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BR2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="BS2" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="BT2" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="BU2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BV2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="BW2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="BX2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="BY2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="BZ2" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="CA2" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="CB2" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="CC2" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="CD2" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="CE2" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="CF2" s="3">
-        <v>2</v>
-      </c>
-      <c r="CG2" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="CH2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="CI2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="CJ2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="CK2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="CL2" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="CM2" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="CN2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="CO2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="CP2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="CQ2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="CR2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="CS2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="CT2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="CU2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="CV2" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="CW2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="CX2" s="3">
-        <v>2</v>
-      </c>
-      <c r="CY2" s="3">
-        <v>1</v>
-      </c>
-      <c r="CZ2" s="3">
-        <v>0</v>
-      </c>
-      <c r="DA2" s="3">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="CX2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="CY2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="CZ2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="DA2" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="DB2" s="3" t="s">
-        <v>174</v>
+        <v>15</v>
       </c>
       <c r="DC2" s="3" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="DD2" s="3" t="s">
-        <v>219</v>
+        <v>59</v>
       </c>
       <c r="DE2" s="3" t="s">
         <v>173</v>
       </c>
       <c r="DF2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="DG2" s="3">
-        <v>30</v>
-      </c>
-      <c r="DH2" s="3">
-        <v>209908</v>
+        <v>11</v>
+      </c>
+      <c r="DG2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="DH2" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="DI2" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="DJ2" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="DK2" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="DL2" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="DM2" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="DN2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="DO2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="DP2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="DQ2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="DR2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="DS2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="DT2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="DU2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="DV2" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="DW2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="DX2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="DY2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="DZ2" s="3" t="s">
         <v>174</v>
       </c>
     </row>
@@ -2986,28 +2755,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD82B76-86B7-46D2-A39A-FB3938032EE5}">
-  <dimension ref="A1:CU2"/>
+  <dimension ref="A1:CD2"/>
   <sheetViews>
-    <sheetView topLeftCell="CH1" workbookViewId="0">
-      <selection activeCell="CQ7" sqref="CQ7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="43" width="22.7109375" style="14"/>
-    <col min="44" max="44" width="47.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="45" max="46" width="22.7109375" style="14"/>
-    <col min="47" max="47" width="30.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="26.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="38.42578125" style="14" customWidth="1"/>
-    <col min="50" max="50" width="37" style="14" customWidth="1"/>
-    <col min="51" max="70" width="22.7109375" style="14"/>
-    <col min="71" max="71" width="41.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="35.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="73" max="16384" width="22.7109375" style="14"/>
+    <col min="1" max="26" width="22.7109375" style="14"/>
+    <col min="27" max="27" width="47.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="22.7109375" style="14"/>
+    <col min="30" max="30" width="30.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="26.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="38.42578125" style="14" customWidth="1"/>
+    <col min="33" max="33" width="37" style="14" customWidth="1"/>
+    <col min="34" max="53" width="22.7109375" style="14"/>
+    <col min="54" max="54" width="41.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="35.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="56" max="16384" width="22.7109375" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>153</v>
       </c>
@@ -3042,275 +2811,224 @@
         <v>159</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>152</v>
+        <v>187</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>14</v>
+        <v>168</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>227</v>
+        <v>170</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>68</v>
+        <v>171</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>70</v>
+        <v>178</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>71</v>
+        <v>179</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>72</v>
+        <v>180</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>228</v>
+        <v>181</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>229</v>
+        <v>182</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>230</v>
+        <v>183</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>232</v>
+        <v>185</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>233</v>
+        <v>186</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>234</v>
+        <v>29</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>187</v>
+        <v>31</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>169</v>
+        <v>250</v>
+      </c>
+      <c r="AE1" s="6" t="s">
+        <v>251</v>
       </c>
       <c r="AF1" s="2" t="s">
-        <v>170</v>
+        <v>125</v>
       </c>
       <c r="AG1" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>179</v>
+        <v>126</v>
+      </c>
+      <c r="AH1" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="AI1" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ1" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="AK1" s="2" t="s">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="AL1" s="2" t="s">
-        <v>181</v>
+        <v>131</v>
       </c>
       <c r="AM1" s="2" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="AN1" s="2" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="AO1" s="2" t="s">
-        <v>184</v>
+        <v>134</v>
       </c>
       <c r="AP1" s="2" t="s">
-        <v>185</v>
+        <v>149</v>
       </c>
       <c r="AQ1" s="2" t="s">
-        <v>186</v>
+        <v>135</v>
       </c>
       <c r="AR1" s="2" t="s">
-        <v>29</v>
+        <v>136</v>
       </c>
       <c r="AS1" s="2" t="s">
-        <v>30</v>
+        <v>137</v>
       </c>
       <c r="AT1" s="2" t="s">
-        <v>31</v>
+        <v>138</v>
       </c>
       <c r="AU1" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="AV1" s="6" t="s">
-        <v>251</v>
+        <v>139</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="AW1" s="2" t="s">
-        <v>125</v>
+        <v>188</v>
       </c>
       <c r="AX1" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="AY1" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="AZ1" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="BA1" s="6" t="s">
-        <v>129</v>
+        <v>189</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="BA1" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="BB1" s="2" t="s">
-        <v>130</v>
+        <v>193</v>
       </c>
       <c r="BC1" s="2" t="s">
-        <v>131</v>
+        <v>194</v>
       </c>
       <c r="BD1" s="2" t="s">
-        <v>132</v>
+        <v>195</v>
       </c>
       <c r="BE1" s="2" t="s">
-        <v>133</v>
+        <v>196</v>
       </c>
       <c r="BF1" s="2" t="s">
-        <v>134</v>
+        <v>197</v>
       </c>
       <c r="BG1" s="2" t="s">
-        <v>149</v>
+        <v>198</v>
       </c>
       <c r="BH1" s="2" t="s">
-        <v>135</v>
+        <v>199</v>
       </c>
       <c r="BI1" s="2" t="s">
-        <v>136</v>
+        <v>200</v>
       </c>
       <c r="BJ1" s="2" t="s">
-        <v>137</v>
+        <v>201</v>
       </c>
       <c r="BK1" s="2" t="s">
-        <v>138</v>
+        <v>202</v>
       </c>
       <c r="BL1" s="2" t="s">
-        <v>139</v>
+        <v>203</v>
       </c>
       <c r="BM1" s="2" t="s">
-        <v>140</v>
+        <v>204</v>
       </c>
       <c r="BN1" s="2" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="BO1" s="2" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
       <c r="BP1" s="2" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c r="BQ1" s="2" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="BR1" s="2" t="s">
-        <v>192</v>
+        <v>209</v>
       </c>
       <c r="BS1" s="2" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
       <c r="BT1" s="2" t="s">
-        <v>194</v>
+        <v>211</v>
       </c>
       <c r="BU1" s="2" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
       <c r="BV1" s="2" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
       <c r="BW1" s="2" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="BX1" s="2" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="BY1" s="2" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
       <c r="BZ1" s="2" t="s">
-        <v>200</v>
+        <v>217</v>
       </c>
       <c r="CA1" s="2" t="s">
-        <v>201</v>
+        <v>75</v>
       </c>
       <c r="CB1" s="2" t="s">
-        <v>202</v>
+        <v>144</v>
       </c>
       <c r="CC1" s="2" t="s">
-        <v>203</v>
+        <v>145</v>
       </c>
       <c r="CD1" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="CE1" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="CF1" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="CG1" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="CH1" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="CI1" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="CJ1" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="CK1" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="CL1" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="CM1" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="CN1" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="CO1" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="CP1" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="CQ1" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="CR1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="CS1" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="CT1" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="CU1" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:99" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:82" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="18" t="s">
         <v>50</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -3340,268 +3058,217 @@
       <c r="K2" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="L2" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>162</v>
       </c>
+      <c r="M2" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="N2" s="3">
+        <v>200</v>
+      </c>
       <c r="O2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>200</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S2" s="3">
+        <v>2</v>
+      </c>
+      <c r="T2" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="P2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="3" t="s">
+      <c r="U2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="W2" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="S2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="U2" s="15" t="s">
-        <v>160</v>
-      </c>
-      <c r="V2" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="X2" s="3" t="s">
-        <v>15</v>
+        <v>175</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>164</v>
+        <v>102</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>165</v>
+        <v>54</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>166</v>
+        <v>55</v>
       </c>
       <c r="AB2" s="3">
         <v>200</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="AD2" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="AE2" s="3">
-        <v>200</v>
+        <v>260</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>147</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>25</v>
+        <v>173</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="AH2" s="3">
-        <v>200</v>
+        <v>174</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>52</v>
+        <v>175</v>
       </c>
       <c r="AJ2" s="3">
         <v>2</v>
       </c>
       <c r="AK2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP2" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AQ2" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AU2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AV2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AW2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AX2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AZ2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="BA2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="BB2" s="18">
+        <v>2</v>
+      </c>
+      <c r="BC2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="BD2" s="18">
+        <v>0</v>
+      </c>
+      <c r="BE2" s="18">
+        <v>0</v>
+      </c>
+      <c r="BF2" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="BG2" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="BH2" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="BI2" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="AM2" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="AP2" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AR2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AS2" s="3">
-        <v>200</v>
-      </c>
-      <c r="AT2" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="AU2" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="AV2" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="AW2" s="3" t="s">
+      <c r="BJ2" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="BK2" s="18">
+        <v>30</v>
+      </c>
+      <c r="BL2" s="18">
+        <v>209908</v>
+      </c>
+      <c r="BM2" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="BN2" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="BO2" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="BP2" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="BQ2" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="BR2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="BS2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="BT2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="BU2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="BV2" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="BW2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="BX2" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="BY2" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="BZ2" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="AX2" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="AY2" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AZ2" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="BA2" s="3">
-        <v>2</v>
-      </c>
-      <c r="BB2" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="BC2" s="3" t="s">
+      <c r="CA2" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="CB2" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="BD2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BE2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BF2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="BG2" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="BH2" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="BI2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BJ2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="BK2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="BL2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="BM2" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="BN2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BO2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BP2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BQ2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BR2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="BS2" s="14">
-        <v>2</v>
-      </c>
-      <c r="BT2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="BU2" s="14">
-        <v>0</v>
-      </c>
-      <c r="BV2" s="14">
-        <v>0</v>
-      </c>
-      <c r="BW2" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="BX2" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="BY2" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="BZ2" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="CA2" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="CB2" s="14">
-        <v>30</v>
-      </c>
-      <c r="CC2" s="14">
-        <v>209908</v>
-      </c>
-      <c r="CD2" s="14" t="s">
-        <v>220</v>
-      </c>
-      <c r="CE2" s="14" t="s">
-        <v>221</v>
-      </c>
-      <c r="CF2" s="14" t="s">
-        <v>222</v>
-      </c>
-      <c r="CG2" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="CH2" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="CI2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="CJ2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="CK2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="CL2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="CM2" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="CN2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="CO2" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="CP2" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="CQ2" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="CR2" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="CS2" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="CT2" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="CU2" s="14" t="s">
+      <c r="CC2" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="CD2" s="18" t="s">
         <v>174</v>
       </c>
     </row>
@@ -3615,8 +3282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C5AC4B7-6134-45E3-A57F-AB8A9E04659F}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>